<commit_message>
Seguimos ajustando apertura V2
</commit_message>
<xml_diff>
--- a/APP_PERSONAS_XML/src/test/resources/datadriven/inversionvirtual/Trn_0325SimulacionIV.xlsx
+++ b/APP_PERSONAS_XML/src/test/resources/datadriven/inversionvirtual/Trn_0325SimulacionIV.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/Documents/Devops/ETC_APP/PITTS_CanalesVirtuales_XML_TEST/src/test/resources/datadriven/virtualinvestment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/Documents/Devops/ETC_APP/nuevaApp/AW1059001_NuevaAPPSucursalVirtualPersonas_Test/APP_PERSONAS_XML/src/test/resources/datadriven/inversionvirtual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C467B020-BDD7-5A4E-87DD-C62F3E1B7833}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C7695E-D0E9-374E-BA9C-64651DA09EFE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>orientacion</t>
   </si>
@@ -185,6 +185,12 @@
   </si>
   <si>
     <t>500000</t>
+  </si>
+  <si>
+    <t>40676340007</t>
+  </si>
+  <si>
+    <t>1035103510</t>
   </si>
 </sst>
 </file>
@@ -604,7 +610,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -678,7 +684,7 @@
         <v>28</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>28</v>
@@ -704,8 +710,8 @@
       <c r="J2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="9">
-        <v>40675536005</v>
+      <c r="K2" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Seguimos ajustando autenticacion V2
</commit_message>
<xml_diff>
--- a/APP_PERSONAS_XML/src/test/resources/datadriven/inversionvirtual/Trn_0325SimulacionIV.xlsx
+++ b/APP_PERSONAS_XML/src/test/resources/datadriven/inversionvirtual/Trn_0325SimulacionIV.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/Documents/Devops/ETC_APP/nuevaApp/AW1059001_NuevaAPPSucursalVirtualPersonas_Test/APP_PERSONAS_XML/src/test/resources/datadriven/inversionvirtual/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AUTOMATIZACION JAVA\PROYECTOS GRADLE\PROYECTOS NUEVA APP\AW1059001_APPSucursalVirtualPersonas_Test\APP_PERSONAS_XML\src\test\resources\datadriven\inversionvirtual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C7695E-D0E9-374E-BA9C-64651DA09EFE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="19455"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -172,9 +171,6 @@
     <t>TasaEfectiva</t>
   </si>
   <si>
-    <t>2.89</t>
-  </si>
-  <si>
     <t>Tiempo</t>
   </si>
   <si>
@@ -191,12 +187,15 @@
   </si>
   <si>
     <t>1035103510</t>
+  </si>
+  <si>
+    <t>4.20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="12"/>
@@ -282,7 +281,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -606,26 +605,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="14.33203125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="11.125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="14.375" style="8" customWidth="1"/>
     <col min="7" max="8" width="11" style="8"/>
-    <col min="9" max="9" width="18.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.375" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.375" style="8" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.5" style="8" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" style="8"/>
-    <col min="14" max="14" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.375" style="8" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.375" style="8" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
@@ -673,7 +672,7 @@
         <v>41</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>44</v>
@@ -684,7 +683,7 @@
         <v>28</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>28</v>
@@ -705,28 +704,28 @@
         <v>5</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>37</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>34</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O2" s="6" t="s">
         <v>42</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="18">
@@ -755,7 +754,7 @@
         <v>5</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>37</v>
@@ -767,16 +766,16 @@
         <v>34</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>43</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -788,15 +787,15 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>G2:G3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'/Users/usuario/Documents/D:\AUTOMATIZACION JAVA\PROYECTOS GRADLE\PROYECTOS XML\PITTS_CanalesVirtuales_XML_TEST\src\test\resources\datadriven\transfers\[Trn_0438-0538TransferenciasBancolombia.xlsx]Listas'!#REF!</xm:f>
+            <xm:f>'\Users\usuario\Documents\D:\AUTOMATIZACION JAVA\PROYECTOS GRADLE\PROYECTOS XML\PITTS_CanalesVirtuales_XML_TEST\src\test\resources\datadriven\transfers\[Trn_0438-0538TransferenciasBancolombia.xlsx]Listas'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>L2:L3</xm:sqref>
         </x14:dataValidation>
@@ -807,19 +806,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>